<commit_message>
Add debugging scripts and enhance cell detection logic
- Introduced `debug_all_sheets.py` to print sheet names and contents from the extracted Excel file.
- Added `debug_cells.py` for detailed processing of PDF pages, including image scaling and table detection.
- Implemented `detect_cells_from_text_positions` in `text_cell_mapper.py` to cluster text positions into table cells.
- Updated `cell_detector.py` to remove wrapper cells that contain multiple smaller cells.
- Enhanced `main.py` with a progress bar for better user feedback during processing.
- Updated `requirements.txt` to include necessary dependencies for new features.
</commit_message>
<xml_diff>
--- a/Output/extracted_output.xlsx
+++ b/Output/extracted_output.xlsx
@@ -9,7 +9,9 @@
   <sheets>
     <sheet name="Page_1_Table_1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Page_2_Table_1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Page_3_Table_1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Page_2_Table_2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Page_3_Table_1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Page_4_Table_1" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,24 +426,124 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr"/>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Subsystem Overview</t>
+        </is>
+      </c>
       <c r="B1" t="inlineStr"/>
       <c r="C1" t="inlineStr"/>
+      <c r="D1" t="inlineStr"/>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Subsystem</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Owner</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Criticality</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Power Management</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Electrical Team</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Voltage sensitive Requires monitoring</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Control Logic</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Firmware Team</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Timing dependent logic</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Thermal</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Mechanical</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Heat dissipation Multi-zone cooling</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Safety</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Compliance</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Regulatory bound Fail-safe required</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -454,7 +556,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,34 +565,92 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr"/>
-      <c r="B1" t="inlineStr"/>
-      <c r="C1" t="inlineStr"/>
-      <c r="D1" t="inlineStr"/>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Parameter</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Min</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Voltage</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>210</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Current</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Frequency</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Hz</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -503,7 +663,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,60 +674,1298 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Cause</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr"/>
-      <c r="C1" t="inlineStr"/>
-      <c r="D1" t="inlineStr"/>
-      <c r="E1" t="inlineStr"/>
-      <c r="F1" t="inlineStr"/>
-      <c r="G1" t="inlineStr"/>
+          <t>Parameter</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Height</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>cm</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Width</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>cm</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr"/>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>E1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>E2</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>E4</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>E5</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>E6</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>E7</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>E8</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>E9</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>E10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>C4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>C5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>C6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>C7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>C8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>C9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>C10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Config A</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Config B</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Config C</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CFG-1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Configuration 1 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CFG-2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Configuration 2 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CFG-3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Configuration 3 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CFG-4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Configuration 4 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CFG-5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Configuration 5 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>CFG-6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Configuration 6 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>CFG-7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Configuration 7 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>CFG-8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Configuration 8 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>CFG-9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Configuration 9 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>CFG-10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Configuration 10 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>CFG-11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Configuration 11 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>CFG-12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Configuration 12 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>CFG-13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Configuration 13 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>CFG-14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Configuration 14 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>CFG-15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Configuration 15 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>CFG-16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Configuration 16 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>CFG-17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Configuration 17 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>CFG-18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Configuration 18 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>CFG-19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Configuration 19 with multiple conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>CFG-20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Configuration 20 with multiple conditions</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>